<commit_message>
Add evidence B6 task
</commit_message>
<xml_diff>
--- a/evidence.xlsx
+++ b/evidence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frkn_\Desktop\gon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6D2C0B-41FE-416B-909B-B91683D3A487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200D78FA-65C9-41C1-AD97-E55F8F0DB2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="1224" windowWidth="16560" windowHeight="10008" firstSheet="14" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="103">
   <si>
     <t>TxHash</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>9B139418B837ADB23F7056ADF9ADEFA6BE7C30053D3D63B6693EB4176EB80638</t>
+  </si>
+  <si>
+    <t>F2D8BB8E9EB930C0E46C330C9C8E4DE3BCE89D7AAC22B606D0EC6EFF0204696F</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1855,9 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>